<commit_message>
Update ONS deaths data (accessed 22 July 2020)
</commit_message>
<xml_diff>
--- a/Data/ONS data/ons-coronavirus-deaths_latest.xlsx
+++ b/Data/ONS data/ons-coronavirus-deaths_latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medkarn_leeds_ac_uk/Documents/Postdoc - Urban Analytics (LIDA)/Research/Covid exponential growth/Data/ONS data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medkarn_leeds_ac_uk/Documents/Postdoc - Urban Analytics (LIDA)/Research/COVID-19/Counterfactual growth (England)/covid-counterfactual/Data/ONS data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{4F0BDF9C-2C9B-5546-935E-2DAAC33ECEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{73030891-3715-0041-B299-684AD455DF3C}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{4F0BDF9C-2C9B-5546-935E-2DAAC33ECEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B18C036-C6A6-7A4C-99E4-55A76CC2D609}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="460" windowWidth="29260" windowHeight="19600" xr2:uid="{9DD6A168-C9F1-FC45-8940-DB034A2E4622}"/>
+    <workbookView xWindow="4940" yWindow="460" windowWidth="29260" windowHeight="19600" xr2:uid="{9DD6A168-C9F1-FC45-8940-DB034A2E4622}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="5">
   <si>
     <t>Area name</t>
   </si>
@@ -101,13 +101,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883200AE-1AA1-F64E-86DA-63CD64FCDD9E}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,12 +455,12 @@
       <c r="B2" s="2">
         <v>43895</v>
       </c>
-      <c r="C2" s="3">
-        <v>5</v>
+      <c r="C2">
+        <v>4</v>
       </c>
       <c r="D2">
         <f>C2</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -471,12 +470,12 @@
       <c r="B3" s="2">
         <v>43896</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>6</v>
       </c>
       <c r="D3">
         <f>C3-C2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -486,7 +485,7 @@
       <c r="B4" s="2">
         <v>43897</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>6</v>
       </c>
       <c r="D4">
@@ -501,7 +500,7 @@
       <c r="B5" s="2">
         <v>43898</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>8</v>
       </c>
       <c r="D5">
@@ -516,7 +515,7 @@
       <c r="B6" s="2">
         <v>43899</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>13</v>
       </c>
       <c r="D6">
@@ -531,12 +530,12 @@
       <c r="B7" s="2">
         <v>43900</v>
       </c>
-      <c r="C7" s="3">
-        <v>15</v>
+      <c r="C7">
+        <v>16</v>
       </c>
       <c r="D7">
         <f>C7-C6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -546,12 +545,12 @@
       <c r="B8" s="2">
         <v>43901</v>
       </c>
-      <c r="C8" s="3">
-        <v>21</v>
+      <c r="C8">
+        <v>23</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D71" si="0">C8-C7</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -561,8 +560,8 @@
       <c r="B9" s="2">
         <v>43902</v>
       </c>
-      <c r="C9" s="3">
-        <v>32</v>
+      <c r="C9">
+        <v>34</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -576,8 +575,8 @@
       <c r="B10" s="2">
         <v>43903</v>
       </c>
-      <c r="C10" s="3">
-        <v>47</v>
+      <c r="C10">
+        <v>49</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -591,8 +590,8 @@
       <c r="B11" s="2">
         <v>43904</v>
       </c>
-      <c r="C11" s="3">
-        <v>66</v>
+      <c r="C11">
+        <v>68</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -606,8 +605,8 @@
       <c r="B12" s="2">
         <v>43905</v>
       </c>
-      <c r="C12" s="3">
-        <v>94</v>
+      <c r="C12">
+        <v>96</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -621,8 +620,8 @@
       <c r="B13" s="2">
         <v>43906</v>
       </c>
-      <c r="C13" s="3">
-        <v>137</v>
+      <c r="C13">
+        <v>139</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -636,12 +635,12 @@
       <c r="B14" s="2">
         <v>43907</v>
       </c>
-      <c r="C14" s="3">
-        <v>189</v>
+      <c r="C14">
+        <v>192</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -651,8 +650,8 @@
       <c r="B15" s="2">
         <v>43908</v>
       </c>
-      <c r="C15" s="3">
-        <v>254</v>
+      <c r="C15">
+        <v>257</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -666,12 +665,12 @@
       <c r="B16" s="2">
         <v>43909</v>
       </c>
-      <c r="C16" s="3">
-        <v>323</v>
+      <c r="C16">
+        <v>327</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -681,8 +680,8 @@
       <c r="B17" s="2">
         <v>43910</v>
       </c>
-      <c r="C17" s="3">
-        <v>429</v>
+      <c r="C17">
+        <v>433</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -696,12 +695,12 @@
       <c r="B18" s="2">
         <v>43911</v>
       </c>
-      <c r="C18" s="3">
-        <v>550</v>
+      <c r="C18">
+        <v>555</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,12 +710,12 @@
       <c r="B19" s="2">
         <v>43912</v>
       </c>
-      <c r="C19" s="3">
-        <v>720</v>
+      <c r="C19">
+        <v>726</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -726,8 +725,8 @@
       <c r="B20" s="2">
         <v>43913</v>
       </c>
-      <c r="C20" s="3">
-        <v>907</v>
+      <c r="C20">
+        <v>913</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -741,12 +740,12 @@
       <c r="B21" s="2">
         <v>43914</v>
       </c>
-      <c r="C21" s="3">
-        <v>1140</v>
+      <c r="C21">
+        <v>1148</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -756,12 +755,12 @@
       <c r="B22" s="2">
         <v>43915</v>
       </c>
-      <c r="C22" s="3">
-        <v>1433</v>
+      <c r="C22">
+        <v>1444</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -771,12 +770,12 @@
       <c r="B23" s="2">
         <v>43916</v>
       </c>
-      <c r="C23" s="3">
-        <v>1801</v>
+      <c r="C23">
+        <v>1813</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -786,12 +785,12 @@
       <c r="B24" s="2">
         <v>43917</v>
       </c>
-      <c r="C24" s="3">
-        <v>2209</v>
+      <c r="C24">
+        <v>2224</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -801,12 +800,12 @@
       <c r="B25" s="2">
         <v>43918</v>
       </c>
-      <c r="C25" s="3">
-        <v>2654</v>
+      <c r="C25">
+        <v>2673</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -816,12 +815,12 @@
       <c r="B26" s="2">
         <v>43919</v>
       </c>
-      <c r="C26" s="3">
-        <v>3177</v>
+      <c r="C26">
+        <v>3202</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>523</v>
+        <v>529</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -831,12 +830,12 @@
       <c r="B27" s="2">
         <v>43920</v>
       </c>
-      <c r="C27" s="3">
-        <v>3793</v>
+      <c r="C27">
+        <v>3827</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>616</v>
+        <v>625</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -846,12 +845,12 @@
       <c r="B28" s="2">
         <v>43921</v>
       </c>
-      <c r="C28" s="3">
-        <v>4527</v>
+      <c r="C28">
+        <v>4565</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>734</v>
+        <v>738</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -861,12 +860,12 @@
       <c r="B29" s="2">
         <v>43922</v>
       </c>
-      <c r="C29" s="3">
-        <v>5339</v>
+      <c r="C29">
+        <v>5383</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>812</v>
+        <v>818</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -876,12 +875,12 @@
       <c r="B30" s="2">
         <v>43923</v>
       </c>
-      <c r="C30" s="3">
-        <v>6224</v>
+      <c r="C30">
+        <v>6271</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>885</v>
+        <v>888</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -891,12 +890,12 @@
       <c r="B31" s="2">
         <v>43924</v>
       </c>
-      <c r="C31" s="3">
-        <v>7138</v>
+      <c r="C31">
+        <v>7192</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>914</v>
+        <v>921</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -906,12 +905,12 @@
       <c r="B32" s="2">
         <v>43925</v>
       </c>
-      <c r="C32" s="3">
-        <v>8142</v>
+      <c r="C32">
+        <v>8207</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>1004</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -921,12 +920,12 @@
       <c r="B33" s="2">
         <v>43926</v>
       </c>
-      <c r="C33" s="3">
-        <v>9195</v>
+      <c r="C33">
+        <v>9265</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>1053</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,12 +935,12 @@
       <c r="B34" s="2">
         <v>43927</v>
       </c>
-      <c r="C34" s="3">
-        <v>10203</v>
+      <c r="C34">
+        <v>10281</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>1008</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -951,12 +950,12 @@
       <c r="B35" s="2">
         <v>43928</v>
       </c>
-      <c r="C35" s="3">
-        <v>11334</v>
+      <c r="C35">
+        <v>11418</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>1131</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -966,12 +965,12 @@
       <c r="B36" s="2">
         <v>43929</v>
       </c>
-      <c r="C36" s="3">
-        <v>12596</v>
+      <c r="C36">
+        <v>12690</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>1262</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -981,12 +980,12 @@
       <c r="B37" s="2">
         <v>43930</v>
       </c>
-      <c r="C37" s="3">
-        <v>13748</v>
+      <c r="C37">
+        <v>13852</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>1152</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -996,12 +995,12 @@
       <c r="B38" s="2">
         <v>43931</v>
       </c>
-      <c r="C38" s="3">
-        <v>14894</v>
+      <c r="C38">
+        <v>15005</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>1146</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1011,12 +1010,12 @@
       <c r="B39" s="2">
         <v>43932</v>
       </c>
-      <c r="C39" s="3">
-        <v>16078</v>
+      <c r="C39">
+        <v>16200</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>1184</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1026,12 +1025,12 @@
       <c r="B40" s="2">
         <v>43933</v>
       </c>
-      <c r="C40" s="3">
-        <v>17264</v>
+      <c r="C40">
+        <v>17391</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>1186</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,12 +1040,12 @@
       <c r="B41" s="2">
         <v>43934</v>
       </c>
-      <c r="C41" s="3">
-        <v>18321</v>
+      <c r="C41">
+        <v>18460</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>1057</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,12 +1055,12 @@
       <c r="B42" s="2">
         <v>43935</v>
       </c>
-      <c r="C42" s="3">
-        <v>19384</v>
+      <c r="C42">
+        <v>19536</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>1063</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1071,12 +1070,12 @@
       <c r="B43" s="2">
         <v>43936</v>
       </c>
-      <c r="C43" s="3">
-        <v>20466</v>
+      <c r="C43">
+        <v>20628</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>1082</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1086,12 +1085,12 @@
       <c r="B44" s="2">
         <v>43937</v>
       </c>
-      <c r="C44" s="3">
-        <v>21593</v>
+      <c r="C44">
+        <v>21764</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>1127</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1101,12 +1100,12 @@
       <c r="B45" s="2">
         <v>43938</v>
       </c>
-      <c r="C45" s="3">
-        <v>22678</v>
+      <c r="C45">
+        <v>22866</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>1085</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1116,12 +1115,12 @@
       <c r="B46" s="2">
         <v>43939</v>
       </c>
-      <c r="C46" s="3">
-        <v>23686</v>
+      <c r="C46">
+        <v>23884</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>1008</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1131,12 +1130,12 @@
       <c r="B47" s="2">
         <v>43940</v>
       </c>
-      <c r="C47" s="3">
-        <v>24644</v>
+      <c r="C47">
+        <v>24850</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>958</v>
+        <v>966</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1146,12 +1145,12 @@
       <c r="B48" s="2">
         <v>43941</v>
       </c>
-      <c r="C48" s="3">
-        <v>25617</v>
+      <c r="C48">
+        <v>25835</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>973</v>
+        <v>985</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,12 +1160,12 @@
       <c r="B49" s="2">
         <v>43942</v>
       </c>
-      <c r="C49" s="3">
-        <v>26513</v>
+      <c r="C49">
+        <v>26742</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>896</v>
+        <v>907</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1176,12 +1175,12 @@
       <c r="B50" s="2">
         <v>43943</v>
       </c>
-      <c r="C50" s="3">
-        <v>27434</v>
+      <c r="C50">
+        <v>27675</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>921</v>
+        <v>933</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1191,12 +1190,12 @@
       <c r="B51" s="2">
         <v>43944</v>
       </c>
-      <c r="C51" s="3">
-        <v>28310</v>
+      <c r="C51">
+        <v>28562</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>876</v>
+        <v>887</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1206,12 +1205,12 @@
       <c r="B52" s="2">
         <v>43945</v>
       </c>
-      <c r="C52" s="3">
-        <v>29163</v>
+      <c r="C52">
+        <v>29427</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>853</v>
+        <v>865</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1221,12 +1220,12 @@
       <c r="B53" s="2">
         <v>43946</v>
       </c>
-      <c r="C53" s="3">
-        <v>29918</v>
+      <c r="C53">
+        <v>30190</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
-        <v>755</v>
+        <v>763</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1236,12 +1235,12 @@
       <c r="B54" s="2">
         <v>43947</v>
       </c>
-      <c r="C54" s="3">
-        <v>30664</v>
+      <c r="C54">
+        <v>30944</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
-        <v>746</v>
+        <v>754</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1251,12 +1250,12 @@
       <c r="B55" s="2">
         <v>43948</v>
       </c>
-      <c r="C55" s="3">
-        <v>31372</v>
+      <c r="C55">
+        <v>31661</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>708</v>
+        <v>717</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,12 +1265,12 @@
       <c r="B56" s="2">
         <v>43949</v>
       </c>
-      <c r="C56" s="3">
-        <v>32055</v>
+      <c r="C56">
+        <v>32356</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>683</v>
+        <v>695</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1281,12 +1280,12 @@
       <c r="B57" s="2">
         <v>43950</v>
       </c>
-      <c r="C57" s="3">
-        <v>32744</v>
+      <c r="C57">
+        <v>33050</v>
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
-        <v>689</v>
+        <v>694</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1296,12 +1295,12 @@
       <c r="B58" s="2">
         <v>43951</v>
       </c>
-      <c r="C58" s="3">
-        <v>33387</v>
+      <c r="C58">
+        <v>33699</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>643</v>
+        <v>649</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1311,12 +1310,12 @@
       <c r="B59" s="2">
         <v>43952</v>
       </c>
-      <c r="C59" s="3">
-        <v>34030</v>
+      <c r="C59">
+        <v>34353</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
-        <v>643</v>
+        <v>654</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1326,12 +1325,12 @@
       <c r="B60" s="2">
         <v>43953</v>
       </c>
-      <c r="C60" s="3">
-        <v>34605</v>
+      <c r="C60">
+        <v>34939</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
-        <v>575</v>
+        <v>586</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1341,12 +1340,12 @@
       <c r="B61" s="2">
         <v>43954</v>
       </c>
-      <c r="C61" s="3">
-        <v>35151</v>
+      <c r="C61">
+        <v>35492</v>
       </c>
       <c r="D61">
         <f t="shared" si="0"/>
-        <v>546</v>
+        <v>553</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1356,12 +1355,12 @@
       <c r="B62" s="2">
         <v>43955</v>
       </c>
-      <c r="C62" s="3">
-        <v>35701</v>
+      <c r="C62">
+        <v>36047</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>555</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1371,12 +1370,12 @@
       <c r="B63" s="2">
         <v>43956</v>
       </c>
-      <c r="C63" s="3">
-        <v>36224</v>
+      <c r="C63">
+        <v>36581</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
-        <v>523</v>
+        <v>534</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1386,12 +1385,12 @@
       <c r="B64" s="2">
         <v>43957</v>
       </c>
-      <c r="C64" s="3">
-        <v>36728</v>
+      <c r="C64">
+        <v>37098</v>
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
-        <v>504</v>
+        <v>517</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1401,12 +1400,12 @@
       <c r="B65" s="2">
         <v>43958</v>
       </c>
-      <c r="C65" s="3">
-        <v>37244</v>
+      <c r="C65">
+        <v>37627</v>
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
-        <v>516</v>
+        <v>529</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,12 +1415,12 @@
       <c r="B66" s="2">
         <v>43959</v>
       </c>
-      <c r="C66" s="3">
-        <v>37715</v>
+      <c r="C66">
+        <v>38103</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1431,12 +1430,12 @@
       <c r="B67" s="2">
         <v>43960</v>
       </c>
-      <c r="C67" s="3">
-        <v>38167</v>
+      <c r="C67">
+        <v>38564</v>
       </c>
       <c r="D67">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1446,12 +1445,12 @@
       <c r="B68" s="2">
         <v>43961</v>
       </c>
-      <c r="C68" s="3">
-        <v>38572</v>
+      <c r="C68">
+        <v>38983</v>
       </c>
       <c r="D68">
         <f t="shared" si="0"/>
-        <v>405</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,12 +1460,12 @@
       <c r="B69" s="2">
         <v>43962</v>
       </c>
-      <c r="C69" s="3">
-        <v>38916</v>
+      <c r="C69">
+        <v>39337</v>
       </c>
       <c r="D69">
         <f t="shared" si="0"/>
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,12 +1475,12 @@
       <c r="B70" s="2">
         <v>43963</v>
       </c>
-      <c r="C70" s="3">
-        <v>39287</v>
+      <c r="C70">
+        <v>39714</v>
       </c>
       <c r="D70">
         <f t="shared" si="0"/>
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1491,12 +1490,12 @@
       <c r="B71" s="2">
         <v>43964</v>
       </c>
-      <c r="C71" s="3">
-        <v>39642</v>
+      <c r="C71">
+        <v>40084</v>
       </c>
       <c r="D71">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1506,12 +1505,12 @@
       <c r="B72" s="2">
         <v>43965</v>
       </c>
-      <c r="C72" s="3">
-        <v>39993</v>
+      <c r="C72">
+        <v>40452</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72:D80" si="1">C72-C71</f>
-        <v>351</v>
+        <f t="shared" ref="D72:D129" si="1">C72-C71</f>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1521,12 +1520,12 @@
       <c r="B73" s="2">
         <v>43966</v>
       </c>
-      <c r="C73" s="3">
-        <v>40336</v>
+      <c r="C73">
+        <v>40807</v>
       </c>
       <c r="D73">
         <f t="shared" si="1"/>
-        <v>343</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1536,12 +1535,12 @@
       <c r="B74" s="2">
         <v>43967</v>
       </c>
-      <c r="C74" s="3">
-        <v>40671</v>
+      <c r="C74">
+        <v>41154</v>
       </c>
       <c r="D74">
         <f t="shared" si="1"/>
-        <v>335</v>
+        <v>347</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1551,12 +1550,12 @@
       <c r="B75" s="2">
         <v>43968</v>
       </c>
-      <c r="C75" s="3">
-        <v>40971</v>
+      <c r="C75">
+        <v>41466</v>
       </c>
       <c r="D75">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1566,12 +1565,12 @@
       <c r="B76" s="2">
         <v>43969</v>
       </c>
-      <c r="C76" s="3">
-        <v>41286</v>
+      <c r="C76">
+        <v>41807</v>
       </c>
       <c r="D76">
         <f t="shared" si="1"/>
-        <v>315</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1581,12 +1580,12 @@
       <c r="B77" s="2">
         <v>43970</v>
       </c>
-      <c r="C77" s="3">
-        <v>41566</v>
+      <c r="C77">
+        <v>42115</v>
       </c>
       <c r="D77">
         <f t="shared" si="1"/>
-        <v>280</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,12 +1595,12 @@
       <c r="B78" s="2">
         <v>43971</v>
       </c>
-      <c r="C78" s="3">
-        <v>41821</v>
+      <c r="C78">
+        <v>42414</v>
       </c>
       <c r="D78">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>299</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1611,12 +1610,12 @@
       <c r="B79" s="2">
         <v>43972</v>
       </c>
-      <c r="C79" s="3">
-        <v>42047</v>
+      <c r="C79">
+        <v>42697</v>
       </c>
       <c r="D79">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1626,12 +1625,747 @@
       <c r="B80" s="2">
         <v>43973</v>
       </c>
-      <c r="C80" s="3">
-        <v>42210</v>
+      <c r="C80">
+        <v>42949</v>
       </c>
       <c r="D80">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="2">
+        <v>43974</v>
+      </c>
+      <c r="C81">
+        <v>43201</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="2">
+        <v>43975</v>
+      </c>
+      <c r="C82">
+        <v>43433</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="2">
+        <v>43976</v>
+      </c>
+      <c r="C83">
+        <v>43667</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="2">
+        <v>43977</v>
+      </c>
+      <c r="C84">
+        <v>43924</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="2">
+        <v>43978</v>
+      </c>
+      <c r="C85">
+        <v>44150</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="2">
+        <v>43979</v>
+      </c>
+      <c r="C86">
+        <v>44385</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="2">
+        <v>43980</v>
+      </c>
+      <c r="C87">
+        <v>44599</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="2">
+        <v>43981</v>
+      </c>
+      <c r="C88">
+        <v>44781</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="2">
+        <v>43982</v>
+      </c>
+      <c r="C89">
+        <v>44953</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="2">
+        <v>43983</v>
+      </c>
+      <c r="C90">
+        <v>45130</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="2">
+        <v>43984</v>
+      </c>
+      <c r="C91">
+        <v>45329</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="2">
+        <v>43985</v>
+      </c>
+      <c r="C92">
+        <v>45504</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="2">
+        <v>43986</v>
+      </c>
+      <c r="C93">
+        <v>45668</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="2">
+        <v>43987</v>
+      </c>
+      <c r="C94">
+        <v>45825</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="2">
+        <v>43988</v>
+      </c>
+      <c r="C95">
+        <v>45946</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="2">
+        <v>43989</v>
+      </c>
+      <c r="C96">
+        <v>46082</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="2">
+        <v>43990</v>
+      </c>
+      <c r="C97">
+        <v>46220</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="2">
+        <v>43991</v>
+      </c>
+      <c r="C98">
+        <v>46347</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="2">
+        <v>43992</v>
+      </c>
+      <c r="C99">
+        <v>46485</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="2">
+        <v>43993</v>
+      </c>
+      <c r="C100">
+        <v>46590</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="2">
+        <v>43994</v>
+      </c>
+      <c r="C101">
+        <v>46707</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="2">
+        <v>43995</v>
+      </c>
+      <c r="C102">
+        <v>46791</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="2">
+        <v>43996</v>
+      </c>
+      <c r="C103">
+        <v>46908</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="2">
+        <v>43997</v>
+      </c>
+      <c r="C104">
+        <v>46996</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="2">
+        <v>43998</v>
+      </c>
+      <c r="C105">
+        <v>47098</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="2">
+        <v>43999</v>
+      </c>
+      <c r="C106">
+        <v>47186</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="2">
+        <v>44000</v>
+      </c>
+      <c r="C107">
+        <v>47263</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="2">
+        <v>44001</v>
+      </c>
+      <c r="C108">
+        <v>47338</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="2">
+        <v>44002</v>
+      </c>
+      <c r="C109">
+        <v>47413</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="2">
+        <v>44003</v>
+      </c>
+      <c r="C110">
+        <v>47478</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="2">
+        <v>44004</v>
+      </c>
+      <c r="C111">
+        <v>47550</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="2">
+        <v>44005</v>
+      </c>
+      <c r="C112">
+        <v>47634</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="2">
+        <v>44006</v>
+      </c>
+      <c r="C113">
+        <v>47723</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="2">
+        <v>44007</v>
+      </c>
+      <c r="C114">
+        <v>47815</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="2">
+        <v>44008</v>
+      </c>
+      <c r="C115">
+        <v>47879</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="2">
+        <v>44009</v>
+      </c>
+      <c r="C116">
+        <v>47937</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="2">
+        <v>44010</v>
+      </c>
+      <c r="C117">
+        <v>47998</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="2">
+        <v>44011</v>
+      </c>
+      <c r="C118">
+        <v>48058</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="2">
+        <v>44012</v>
+      </c>
+      <c r="C119">
+        <v>48126</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="2">
+        <v>44013</v>
+      </c>
+      <c r="C120">
+        <v>48169</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="2">
+        <v>44014</v>
+      </c>
+      <c r="C121">
+        <v>48224</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="2">
+        <v>44015</v>
+      </c>
+      <c r="C122">
+        <v>48267</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="2">
+        <v>44016</v>
+      </c>
+      <c r="C123">
+        <v>48311</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="2">
+        <v>44017</v>
+      </c>
+      <c r="C124">
+        <v>48351</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="2">
+        <v>44018</v>
+      </c>
+      <c r="C125">
+        <v>48393</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="2">
+        <v>44019</v>
+      </c>
+      <c r="C126">
+        <v>48428</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="2">
+        <v>44020</v>
+      </c>
+      <c r="C127">
+        <v>48464</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="2">
+        <v>44021</v>
+      </c>
+      <c r="C128">
+        <v>48506</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="2">
+        <v>44022</v>
+      </c>
+      <c r="C129">
+        <v>48532</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>